<commit_message>
chore(runtime): publish files + archive (2025-11-15 15:05:59)
</commit_message>
<xml_diff>
--- a/khl/Form-5_Games_home_away.xlsx
+++ b/khl/Form-5_Games_home_away.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AH31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,92 +609,92 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Трактор</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>897753</v>
+        <v>897712</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897753.html</t>
+          <t>https://text.khl.ru/text/897712.html</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I2" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J2" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="K2" t="n">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N2" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="O2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P2" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q2" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="R2" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="S2" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="T2" t="n">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="U2" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="V2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X2" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="Y2" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="Z2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
@@ -702,124 +702,124 @@
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>47.8</v>
+        <v>43.7</v>
       </c>
       <c r="AD2" t="n">
-        <v>57.7</v>
+        <v>52.2</v>
       </c>
       <c r="AE2" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AF2" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AG2" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="AH2" t="n">
-        <v>3.1</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Авангард</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>897741</v>
+        <v>897707</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897741.html</t>
+          <t>https://text.khl.ru/text/897707.html</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I3" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="J3" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K3" t="n">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O3" t="n">
         <v>6</v>
       </c>
       <c r="P3" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q3" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R3" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="S3" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="T3" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="U3" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="V3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X3" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Y3" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="Z3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA3" t="n">
         <v>2</v>
       </c>
-      <c r="AA3" t="n">
-        <v>4</v>
-      </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>47.4</v>
+        <v>45.6</v>
       </c>
       <c r="AD3" t="n">
-        <v>58.3</v>
+        <v>41.9</v>
       </c>
       <c r="AE3" t="n">
         <v>0</v>
@@ -828,10 +828,10 @@
         <v>0</v>
       </c>
       <c r="AG3" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AH3" t="n">
-        <v>4</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="4">
@@ -842,12 +842,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Барыс</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Нефтехимик</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Барыс</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -859,19 +859,19 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
         <v>3</v>
       </c>
-      <c r="H4" t="n">
-        <v>2</v>
-      </c>
       <c r="I4" t="n">
+        <v>32</v>
+      </c>
+      <c r="J4" t="n">
         <v>34</v>
-      </c>
-      <c r="J4" t="n">
-        <v>32</v>
       </c>
       <c r="K4" t="n">
         <v>66</v>
@@ -883,57 +883,57 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" t="n">
         <v>6</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
+        <v>41</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>31</v>
+      </c>
+      <c r="R4" t="n">
+        <v>10</v>
+      </c>
+      <c r="S4" t="n">
+        <v>27</v>
+      </c>
+      <c r="T4" t="n">
+        <v>34</v>
+      </c>
+      <c r="U4" t="n">
+        <v>19</v>
+      </c>
+      <c r="V4" t="n">
         <v>4</v>
       </c>
-      <c r="P4" t="n">
-        <v>31</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>41</v>
-      </c>
-      <c r="R4" t="n">
-        <v>27</v>
-      </c>
-      <c r="S4" t="n">
-        <v>10</v>
-      </c>
-      <c r="T4" t="n">
-        <v>19</v>
-      </c>
-      <c r="U4" t="n">
-        <v>34</v>
-      </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>5</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z4" t="n">
         <v>4</v>
       </c>
-      <c r="X4" t="n">
-        <v>18</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>23</v>
-      </c>
-      <c r="Z4" t="n">
+      <c r="AA4" t="n">
         <v>3</v>
       </c>
-      <c r="AA4" t="n">
-        <v>4</v>
-      </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>43.1</v>
+        <v>56.9</v>
       </c>
       <c r="AD4" t="n">
-        <v>35.8</v>
+        <v>64.2</v>
       </c>
       <c r="AE4" t="n">
         <v>0</v>
@@ -945,98 +945,98 @@
         <v>1</v>
       </c>
       <c r="AH4" t="n">
-        <v>8.800000000000001</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Трактор</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>897689</v>
+        <v>897628</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897689.html</t>
+          <t>https://text.khl.ru/text/897628.html</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J5" t="n">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="K5" t="n">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
+        <v>13</v>
+      </c>
+      <c r="O5" t="n">
         <v>12</v>
       </c>
-      <c r="O5" t="n">
-        <v>4</v>
-      </c>
       <c r="P5" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="Q5" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="R5" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="S5" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T5" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="U5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="V5" t="n">
         <v>5</v>
       </c>
       <c r="W5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="X5" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Y5" t="n">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="Z5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
@@ -1044,124 +1044,124 @@
         </is>
       </c>
       <c r="AC5" t="n">
-        <v>46.2</v>
+        <v>47.9</v>
       </c>
       <c r="AD5" t="n">
-        <v>58.3</v>
+        <v>40.9</v>
       </c>
       <c r="AE5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="AH5" t="n">
-        <v>4.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>897683</v>
+        <v>897621</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897683.html</t>
+          <t>https://text.khl.ru/text/897621.html</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6" t="n">
+        <v>37</v>
+      </c>
+      <c r="J6" t="n">
+        <v>28</v>
+      </c>
+      <c r="K6" t="n">
+        <v>65</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>8</v>
+      </c>
+      <c r="O6" t="n">
+        <v>8</v>
+      </c>
+      <c r="P6" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>38</v>
+      </c>
+      <c r="R6" t="n">
+        <v>24</v>
+      </c>
+      <c r="S6" t="n">
+        <v>10</v>
+      </c>
+      <c r="T6" t="n">
+        <v>19</v>
+      </c>
+      <c r="U6" t="n">
         <v>23</v>
       </c>
-      <c r="J6" t="n">
-        <v>41</v>
-      </c>
-      <c r="K6" t="n">
-        <v>64</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
+      <c r="V6" t="n">
+        <v>4</v>
+      </c>
+      <c r="W6" t="n">
+        <v>4</v>
+      </c>
+      <c r="X6" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA6" t="n">
         <v>2</v>
       </c>
-      <c r="N6" t="n">
-        <v>12</v>
-      </c>
-      <c r="O6" t="n">
-        <v>16</v>
-      </c>
-      <c r="P6" t="n">
-        <v>36</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>26</v>
-      </c>
-      <c r="R6" t="n">
-        <v>26</v>
-      </c>
-      <c r="S6" t="n">
-        <v>7</v>
-      </c>
-      <c r="T6" t="n">
-        <v>23</v>
-      </c>
-      <c r="U6" t="n">
-        <v>17</v>
-      </c>
-      <c r="V6" t="n">
-        <v>1</v>
-      </c>
-      <c r="W6" t="n">
-        <v>3</v>
-      </c>
-      <c r="X6" t="n">
-        <v>18</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>16</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>3</v>
-      </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>58.1</v>
+        <v>32.1</v>
       </c>
       <c r="AD6" t="n">
-        <v>57.5</v>
+        <v>45.2</v>
       </c>
       <c r="AE6" t="n">
         <v>0</v>
@@ -1170,185 +1170,185 @@
         <v>0</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="AH6" t="n">
-        <v>21.7</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>897758</v>
+        <v>897768</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897758.html</t>
+          <t>https://text.khl.ru/text/897768.html</t>
         </is>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>27</v>
+      </c>
+      <c r="J7" t="n">
+        <v>33</v>
+      </c>
+      <c r="K7" t="n">
+        <v>60</v>
+      </c>
+      <c r="L7" t="n">
+        <v>3</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
         <v>2</v>
       </c>
-      <c r="I7" t="n">
-        <v>34</v>
-      </c>
-      <c r="J7" t="n">
-        <v>27</v>
-      </c>
-      <c r="K7" t="n">
-        <v>61</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>4</v>
-      </c>
       <c r="O7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P7" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="Q7" t="n">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="R7" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S7" t="n">
+        <v>8</v>
+      </c>
+      <c r="T7" t="n">
         <v>20</v>
       </c>
-      <c r="T7" t="n">
-        <v>6</v>
-      </c>
       <c r="U7" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="V7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X7" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="Y7" t="n">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Z7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA7" t="n">
         <v>2</v>
       </c>
-      <c r="AA7" t="n">
-        <v>7</v>
-      </c>
       <c r="AB7" t="inlineStr">
         <is>
           <t>L</t>
         </is>
       </c>
       <c r="AC7" t="n">
-        <v>53.8</v>
+        <v>40.7</v>
       </c>
       <c r="AD7" t="n">
-        <v>30</v>
+        <v>47.6</v>
       </c>
       <c r="AE7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7" t="n">
-        <v>0</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>897744</v>
+        <v>897726</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897744.html</t>
+          <t>https://text.khl.ru/text/897726.html</t>
         </is>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
         <v>36</v>
       </c>
       <c r="J8" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="K8" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O8" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P8" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="Q8" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="R8" t="n">
         <v>19</v>
@@ -1357,28 +1357,28 @@
         <v>11</v>
       </c>
       <c r="T8" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U8" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="V8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W8" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X8" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Y8" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Z8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
@@ -1386,10 +1386,10 @@
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>39.7</v>
+        <v>50</v>
       </c>
       <c r="AD8" t="n">
-        <v>23.7</v>
+        <v>47.2</v>
       </c>
       <c r="AE8" t="n">
         <v>0</v>
@@ -1397,213 +1397,216 @@
       <c r="AF8" t="n">
         <v>0</v>
       </c>
+      <c r="AG8" t="n">
+        <v>0.5</v>
+      </c>
       <c r="AH8" t="n">
-        <v>11.1</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Динамо М</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>Северсталь</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>ХК Сочи</t>
-        </is>
-      </c>
       <c r="D9" t="n">
-        <v>897739</v>
+        <v>897708</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897739.html</t>
+          <t>https://text.khl.ru/text/897708.html</t>
         </is>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14</v>
+      </c>
+      <c r="J9" t="n">
+        <v>22</v>
+      </c>
+      <c r="K9" t="n">
+        <v>36</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>20</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>28</v>
+      </c>
+      <c r="R9" t="n">
+        <v>28</v>
+      </c>
+      <c r="S9" t="n">
+        <v>6</v>
+      </c>
+      <c r="T9" t="n">
+        <v>28</v>
+      </c>
+      <c r="U9" t="n">
+        <v>2</v>
+      </c>
+      <c r="V9" t="n">
+        <v>3</v>
+      </c>
+      <c r="W9" t="n">
         <v>5</v>
       </c>
-      <c r="H9" t="n">
-        <v>4</v>
-      </c>
-      <c r="I9" t="n">
-        <v>37</v>
-      </c>
-      <c r="J9" t="n">
-        <v>19</v>
-      </c>
-      <c r="K9" t="n">
-        <v>56</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" t="n">
-        <v>2</v>
-      </c>
-      <c r="O9" t="n">
-        <v>8</v>
-      </c>
-      <c r="P9" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>26</v>
-      </c>
-      <c r="R9" t="n">
+      <c r="X9" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA9" t="n">
         <v>9</v>
       </c>
-      <c r="S9" t="n">
-        <v>14</v>
-      </c>
-      <c r="T9" t="n">
-        <v>10</v>
-      </c>
-      <c r="U9" t="n">
-        <v>33</v>
-      </c>
-      <c r="V9" t="n">
-        <v>8</v>
-      </c>
-      <c r="W9" t="n">
-        <v>10</v>
-      </c>
-      <c r="X9" t="n">
-        <v>26</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>24</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>4</v>
-      </c>
       <c r="AB9" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
       <c r="AC9" t="n">
-        <v>52.7</v>
+        <v>50</v>
       </c>
       <c r="AD9" t="n">
-        <v>23.3</v>
+        <v>93.3</v>
       </c>
       <c r="AE9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AG9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9" t="n">
-        <v>13.5</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>897681</v>
+        <v>897701</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897681.html</t>
+          <t>https://text.khl.ru/text/897701.html</t>
         </is>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="J10" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K10" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="O10" t="n">
         <v>8</v>
       </c>
       <c r="P10" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q10" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="R10" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="S10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T10" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="U10" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="V10" t="n">
         <v>1</v>
       </c>
       <c r="W10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X10" t="n">
         <v>33</v>
       </c>
       <c r="Y10" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="Z10" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AA10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
@@ -1611,113 +1614,113 @@
         </is>
       </c>
       <c r="AC10" t="n">
-        <v>48</v>
+        <v>59.2</v>
       </c>
       <c r="AD10" t="n">
-        <v>10</v>
+        <v>40.8</v>
       </c>
       <c r="AE10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AH10" t="n">
-        <v>14.8</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>897674</v>
+        <v>897680</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897674.html</t>
+          <t>https://text.khl.ru/text/897680.html</t>
         </is>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="J11" t="n">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="K11" t="n">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="O11" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="P11" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="Q11" t="n">
         <v>27</v>
       </c>
       <c r="R11" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="S11" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="T11" t="n">
+        <v>24</v>
+      </c>
+      <c r="U11" t="n">
+        <v>28</v>
+      </c>
+      <c r="V11" t="n">
+        <v>4</v>
+      </c>
+      <c r="W11" t="n">
         <v>6</v>
       </c>
-      <c r="U11" t="n">
-        <v>16</v>
-      </c>
-      <c r="V11" t="n">
-        <v>5</v>
-      </c>
-      <c r="W11" t="n">
+      <c r="X11" t="n">
+        <v>43</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z11" t="n">
         <v>2</v>
       </c>
-      <c r="X11" t="n">
-        <v>16</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>14</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>7</v>
-      </c>
       <c r="AA11" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
@@ -1725,455 +1728,449 @@
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>51.8</v>
+        <v>56.5</v>
       </c>
       <c r="AD11" t="n">
-        <v>27.3</v>
+        <v>46.2</v>
       </c>
       <c r="AE11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF11" t="n">
-        <v>0</v>
+        <v>0.29</v>
       </c>
       <c r="AG11" t="n">
         <v>1</v>
       </c>
       <c r="AH11" t="n">
-        <v>16</v>
+        <v>27.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>897762</v>
+        <v>897759</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897762.html</t>
+          <t>https://text.khl.ru/text/897759.html</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H12" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J12" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K12" t="n">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="O12" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q12" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="R12" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="S12" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="T12" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="U12" t="n">
         <v>17</v>
       </c>
       <c r="V12" t="n">
+        <v>4</v>
+      </c>
+      <c r="W12" t="n">
         <v>2</v>
       </c>
-      <c r="W12" t="n">
-        <v>3</v>
-      </c>
       <c r="X12" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="Y12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Z12" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA12" t="n">
         <v>4</v>
       </c>
-      <c r="AA12" t="n">
-        <v>1</v>
-      </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>41.9</v>
+        <v>45.3</v>
       </c>
       <c r="AD12" t="n">
-        <v>55.3</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>0.1</v>
+        <v>48.5</v>
       </c>
       <c r="AG12" t="n">
         <v>1</v>
       </c>
       <c r="AH12" t="n">
-        <v>11.1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>897752</v>
+        <v>897730</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897752.html</t>
+          <t>https://text.khl.ru/text/897730.html</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H13" t="n">
         <v>3</v>
       </c>
       <c r="I13" t="n">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="J13" t="n">
+        <v>39</v>
+      </c>
+      <c r="K13" t="n">
+        <v>64</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>16</v>
+      </c>
+      <c r="O13" t="n">
+        <v>14</v>
+      </c>
+      <c r="P13" t="n">
         <v>25</v>
       </c>
-      <c r="K13" t="n">
-        <v>71</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" t="n">
-        <v>10</v>
-      </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
+        <v>34</v>
+      </c>
+      <c r="R13" t="n">
+        <v>16</v>
+      </c>
+      <c r="S13" t="n">
+        <v>9</v>
+      </c>
+      <c r="T13" t="n">
+        <v>11</v>
+      </c>
+      <c r="U13" t="n">
         <v>6</v>
       </c>
-      <c r="P13" t="n">
+      <c r="V13" t="n">
+        <v>5</v>
+      </c>
+      <c r="W13" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" t="n">
         <v>34</v>
       </c>
-      <c r="Q13" t="n">
-        <v>25</v>
-      </c>
-      <c r="R13" t="n">
-        <v>15</v>
-      </c>
-      <c r="S13" t="n">
-        <v>23</v>
-      </c>
-      <c r="T13" t="n">
-        <v>10</v>
-      </c>
-      <c r="U13" t="n">
-        <v>8</v>
-      </c>
-      <c r="V13" t="n">
-        <v>3</v>
-      </c>
-      <c r="W13" t="n">
-        <v>1</v>
-      </c>
-      <c r="X13" t="n">
-        <v>16</v>
-      </c>
       <c r="Y13" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="Z13" t="n">
         <v>3</v>
       </c>
       <c r="AA13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC13" t="n">
-        <v>57.6</v>
+        <v>42.4</v>
       </c>
       <c r="AD13" t="n">
-        <v>55.6</v>
+        <v>64.7</v>
       </c>
       <c r="AE13" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="AF13" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.8</v>
+        <v>0.88</v>
       </c>
       <c r="AH13" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Металлург Мг</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>897699</v>
+        <v>897725</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897699.html</t>
+          <t>https://text.khl.ru/text/897725.html</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
+        <v>6</v>
+      </c>
+      <c r="I14" t="n">
+        <v>24</v>
+      </c>
+      <c r="J14" t="n">
+        <v>44</v>
+      </c>
+      <c r="K14" t="n">
+        <v>68</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
         <v>2</v>
       </c>
-      <c r="I14" t="n">
-        <v>20</v>
-      </c>
-      <c r="J14" t="n">
-        <v>26</v>
-      </c>
-      <c r="K14" t="n">
-        <v>46</v>
-      </c>
-      <c r="L14" t="n">
-        <v>3</v>
-      </c>
-      <c r="M14" t="n">
-        <v>1</v>
-      </c>
       <c r="N14" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O14" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P14" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="Q14" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R14" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="S14" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T14" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="U14" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="V14" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="W14" t="n">
         <v>5</v>
       </c>
       <c r="X14" t="n">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="Y14" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Z14" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="AA14" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>53.2</v>
+        <v>42.6</v>
       </c>
       <c r="AD14" t="n">
-        <v>59.3</v>
+        <v>67.5</v>
       </c>
       <c r="AE14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG14" t="n">
         <v>0.6</v>
       </c>
-      <c r="AG14" t="n">
-        <v>0.67</v>
-      </c>
       <c r="AH14" t="n">
-        <v>15</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ХК Сочи</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>897694</v>
+        <v>897717</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897694.html</t>
+          <t>https://text.khl.ru/text/897717.html</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" t="n">
         <v>3</v>
       </c>
       <c r="I15" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="J15" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="K15" t="n">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="L15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
         <v>6</v>
       </c>
       <c r="O15" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P15" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q15" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="R15" t="n">
+        <v>18</v>
+      </c>
+      <c r="S15" t="n">
+        <v>16</v>
+      </c>
+      <c r="T15" t="n">
+        <v>28</v>
+      </c>
+      <c r="U15" t="n">
         <v>14</v>
       </c>
-      <c r="S15" t="n">
-        <v>21</v>
-      </c>
-      <c r="T15" t="n">
-        <v>10</v>
-      </c>
-      <c r="U15" t="n">
-        <v>23</v>
-      </c>
       <c r="V15" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X15" t="n">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="Y15" t="n">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="Z15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AA15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB15" t="inlineStr">
         <is>
@@ -2181,65 +2178,65 @@
         </is>
       </c>
       <c r="AC15" t="n">
-        <v>45.6</v>
+        <v>46.4</v>
       </c>
       <c r="AD15" t="n">
-        <v>30.3</v>
+        <v>66.7</v>
       </c>
       <c r="AE15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AG15" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="AH15" t="n">
-        <v>11.9</v>
+        <v>26.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>897680</v>
+        <v>897693</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897680.html</t>
+          <t>https://text.khl.ru/text/897693.html</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I16" t="n">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="J16" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="K16" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -2248,46 +2245,46 @@
         <v>2</v>
       </c>
       <c r="N16" t="n">
+        <v>10</v>
+      </c>
+      <c r="O16" t="n">
+        <v>10</v>
+      </c>
+      <c r="P16" t="n">
         <v>14</v>
       </c>
-      <c r="O16" t="n">
-        <v>14</v>
-      </c>
-      <c r="P16" t="n">
-        <v>27</v>
-      </c>
       <c r="Q16" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="R16" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S16" t="n">
         <v>22</v>
       </c>
       <c r="T16" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="U16" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="V16" t="n">
+        <v>2</v>
+      </c>
+      <c r="W16" t="n">
+        <v>1</v>
+      </c>
+      <c r="X16" t="n">
         <v>6</v>
       </c>
-      <c r="W16" t="n">
-        <v>4</v>
-      </c>
-      <c r="X16" t="n">
-        <v>26</v>
-      </c>
       <c r="Y16" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="Z16" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AA16" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AB16" t="inlineStr">
         <is>
@@ -2295,10 +2292,10 @@
         </is>
       </c>
       <c r="AC16" t="n">
-        <v>43.5</v>
+        <v>31.1</v>
       </c>
       <c r="AD16" t="n">
-        <v>53.8</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="AE16" t="n">
         <v>0</v>
@@ -2307,112 +2304,112 @@
         <v>0</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.71</v>
+        <v>0.6</v>
       </c>
       <c r="AH16" t="n">
-        <v>0</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>897724</v>
+        <v>897745</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897724.html</t>
+          <t>https://text.khl.ru/text/897745.html</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J17" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="K17" t="n">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O17" t="n">
         <v>6</v>
       </c>
       <c r="P17" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="Q17" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="R17" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="S17" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T17" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="U17" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="V17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X17" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="Y17" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="Z17" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AA17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>54.5</v>
+        <v>57.8</v>
       </c>
       <c r="AD17" t="n">
-        <v>42.9</v>
+        <v>61.4</v>
       </c>
       <c r="AE17" t="n">
         <v>0</v>
@@ -2421,340 +2418,340 @@
         <v>0</v>
       </c>
       <c r="AG17" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH17" t="n">
-        <v>0</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>897715</v>
+        <v>897737</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897715.html</t>
+          <t>https://text.khl.ru/text/897737.html</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="n">
+        <v>5</v>
+      </c>
+      <c r="H18" t="n">
         <v>2</v>
       </c>
-      <c r="H18" t="n">
-        <v>3</v>
-      </c>
       <c r="I18" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="J18" t="n">
+        <v>29</v>
+      </c>
+      <c r="K18" t="n">
+        <v>56</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" t="n">
+        <v>8</v>
+      </c>
+      <c r="O18" t="n">
+        <v>6</v>
+      </c>
+      <c r="P18" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q18" t="n">
         <v>24</v>
       </c>
-      <c r="K18" t="n">
-        <v>43</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>2</v>
-      </c>
-      <c r="O18" t="n">
-        <v>4</v>
-      </c>
-      <c r="P18" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
+        <v>12</v>
+      </c>
+      <c r="S18" t="n">
+        <v>15</v>
+      </c>
+      <c r="T18" t="n">
         <v>22</v>
       </c>
-      <c r="R18" t="n">
-        <v>20</v>
-      </c>
-      <c r="S18" t="n">
-        <v>21</v>
-      </c>
-      <c r="T18" t="n">
-        <v>11</v>
-      </c>
       <c r="U18" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="V18" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="W18" t="n">
         <v>3</v>
       </c>
       <c r="X18" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="Y18" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="Z18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC18" t="n">
-        <v>52.2</v>
+        <v>53.8</v>
       </c>
       <c r="AD18" t="n">
-        <v>40.7</v>
+        <v>48.9</v>
       </c>
       <c r="AE18" t="n">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="AG18" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AH18" t="n">
-        <v>10.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>СКА</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>897699</v>
+        <v>897664</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897699.html</t>
+          <t>https://text.khl.ru/text/897664.html</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
+        <v>3</v>
+      </c>
+      <c r="H19" t="n">
         <v>2</v>
       </c>
-      <c r="H19" t="n">
-        <v>3</v>
-      </c>
       <c r="I19" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="J19" t="n">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="K19" t="n">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="L19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N19" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O19" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P19" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="Q19" t="n">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="R19" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="S19" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="T19" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="U19" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="V19" t="n">
         <v>5</v>
       </c>
       <c r="W19" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>31</v>
+      </c>
+      <c r="Z19" t="n">
         <v>5</v>
       </c>
-      <c r="X19" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>39</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>2</v>
-      </c>
       <c r="AA19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>46.8</v>
+        <v>60</v>
       </c>
       <c r="AD19" t="n">
-        <v>40.7</v>
+        <v>56.2</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AH19" t="n">
-        <v>7.7</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Лада</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>897676</v>
+        <v>897700</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897676.html</t>
+          <t>https://text.khl.ru/text/897700.html</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J20" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K20" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N20" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O20" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P20" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="Q20" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="R20" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="S20" t="n">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="T20" t="n">
         <v>20</v>
       </c>
       <c r="U20" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="V20" t="n">
+        <v>6</v>
+      </c>
+      <c r="W20" t="n">
+        <v>4</v>
+      </c>
+      <c r="X20" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>52</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA20" t="n">
         <v>3</v>
       </c>
-      <c r="W20" t="n">
-        <v>3</v>
-      </c>
-      <c r="X20" t="n">
-        <v>17</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>33</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA20" t="n">
-        <v>2</v>
-      </c>
       <c r="AB20" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
       <c r="AC20" t="n">
-        <v>44.9</v>
+        <v>68.5</v>
       </c>
       <c r="AD20" t="n">
-        <v>54.1</v>
+        <v>58.8</v>
       </c>
       <c r="AE20" t="n">
         <v>0</v>
@@ -2763,56 +2760,56 @@
         <v>0</v>
       </c>
       <c r="AG20" t="n">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="AH20" t="n">
-        <v>11.8</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>Локомотив</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>ЦСКА</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Торпедо</t>
-        </is>
-      </c>
       <c r="D21" t="n">
-        <v>897660</v>
+        <v>897651</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897660.html</t>
+          <t>https://text.khl.ru/text/897651.html</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J21" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="K21" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
@@ -2821,66 +2818,1200 @@
         <v>2</v>
       </c>
       <c r="O21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P21" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q21" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="R21" t="n">
         <v>16</v>
       </c>
       <c r="S21" t="n">
+        <v>25</v>
+      </c>
+      <c r="T21" t="n">
+        <v>29</v>
+      </c>
+      <c r="U21" t="n">
+        <v>33</v>
+      </c>
+      <c r="V21" t="n">
+        <v>3</v>
+      </c>
+      <c r="W21" t="n">
+        <v>2</v>
+      </c>
+      <c r="X21" t="n">
+        <v>26</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="AC21" t="n">
+        <v>50</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>46.8</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>04-11-2025</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Торпедо</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>897728</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897728.html</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3</v>
+      </c>
+      <c r="I22" t="n">
+        <v>25</v>
+      </c>
+      <c r="J22" t="n">
+        <v>39</v>
+      </c>
+      <c r="K22" t="n">
+        <v>64</v>
+      </c>
+      <c r="L22" t="n">
+        <v>2</v>
+      </c>
+      <c r="M22" t="n">
+        <v>2</v>
+      </c>
+      <c r="N22" t="n">
+        <v>12</v>
+      </c>
+      <c r="O22" t="n">
+        <v>6</v>
+      </c>
+      <c r="P22" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>42</v>
+      </c>
+      <c r="R22" t="n">
+        <v>23</v>
+      </c>
+      <c r="S22" t="n">
+        <v>8</v>
+      </c>
+      <c r="T22" t="n">
+        <v>12</v>
+      </c>
+      <c r="U22" t="n">
+        <v>20</v>
+      </c>
+      <c r="V22" t="n">
+        <v>4</v>
+      </c>
+      <c r="W22" t="n">
+        <v>3</v>
+      </c>
+      <c r="X22" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC22" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>25-10-2025</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Трактор</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>897688</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897688.html</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3</v>
+      </c>
+      <c r="H23" t="n">
+        <v>3</v>
+      </c>
+      <c r="I23" t="n">
+        <v>40</v>
+      </c>
+      <c r="J23" t="n">
+        <v>39</v>
+      </c>
+      <c r="K23" t="n">
+        <v>79</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>4</v>
+      </c>
+      <c r="O23" t="n">
+        <v>7</v>
+      </c>
+      <c r="P23" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>28</v>
+      </c>
+      <c r="R23" t="n">
+        <v>16</v>
+      </c>
+      <c r="S23" t="n">
+        <v>21</v>
+      </c>
+      <c r="T23" t="n">
+        <v>18</v>
+      </c>
+      <c r="U23" t="n">
+        <v>24</v>
+      </c>
+      <c r="V23" t="n">
+        <v>2</v>
+      </c>
+      <c r="W23" t="n">
+        <v>5</v>
+      </c>
+      <c r="X23" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC23" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23-10-2025</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Салават Юлаев</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>897679</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897679.html</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" t="n">
+        <v>5</v>
+      </c>
+      <c r="I24" t="n">
+        <v>22</v>
+      </c>
+      <c r="J24" t="n">
+        <v>45</v>
+      </c>
+      <c r="K24" t="n">
+        <v>67</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" t="n">
+        <v>6</v>
+      </c>
+      <c r="O24" t="n">
+        <v>6</v>
+      </c>
+      <c r="P24" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>28</v>
+      </c>
+      <c r="R24" t="n">
+        <v>12</v>
+      </c>
+      <c r="S24" t="n">
+        <v>18</v>
+      </c>
+      <c r="T24" t="n">
+        <v>15</v>
+      </c>
+      <c r="U24" t="n">
+        <v>9</v>
+      </c>
+      <c r="V24" t="n">
+        <v>7</v>
+      </c>
+      <c r="W24" t="n">
+        <v>2</v>
+      </c>
+      <c r="X24" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y24" t="n">
         <v>11</v>
       </c>
-      <c r="T21" t="n">
-        <v>28</v>
-      </c>
-      <c r="U21" t="n">
+      <c r="Z24" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC24" t="n">
+        <v>50</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>21-10-2025</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Металлург Мг</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>897671</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897671.html</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" t="n">
+        <v>24</v>
+      </c>
+      <c r="J25" t="n">
+        <v>31</v>
+      </c>
+      <c r="K25" t="n">
+        <v>55</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" t="n">
+        <v>2</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>30</v>
+      </c>
+      <c r="R25" t="n">
+        <v>12</v>
+      </c>
+      <c r="S25" t="n">
+        <v>17</v>
+      </c>
+      <c r="T25" t="n">
+        <v>22</v>
+      </c>
+      <c r="U25" t="n">
+        <v>12</v>
+      </c>
+      <c r="V25" t="n">
+        <v>2</v>
+      </c>
+      <c r="W25" t="n">
+        <v>1</v>
+      </c>
+      <c r="X25" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC25" t="n">
+        <v>38.8</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>64.7</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>16-10-2025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Ак Барс</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>897654</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897654.html</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>4</v>
+      </c>
+      <c r="I26" t="n">
         <v>20</v>
       </c>
-      <c r="V21" t="n">
-        <v>7</v>
-      </c>
-      <c r="W21" t="n">
+      <c r="J26" t="n">
+        <v>49</v>
+      </c>
+      <c r="K26" t="n">
+        <v>69</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1</v>
+      </c>
+      <c r="N26" t="n">
+        <v>10</v>
+      </c>
+      <c r="O26" t="n">
+        <v>2</v>
+      </c>
+      <c r="P26" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>29</v>
+      </c>
+      <c r="R26" t="n">
+        <v>20</v>
+      </c>
+      <c r="S26" t="n">
+        <v>10</v>
+      </c>
+      <c r="T26" t="n">
+        <v>16</v>
+      </c>
+      <c r="U26" t="n">
+        <v>16</v>
+      </c>
+      <c r="V26" t="n">
+        <v>3</v>
+      </c>
+      <c r="W26" t="n">
+        <v>4</v>
+      </c>
+      <c r="X26" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC26" t="n">
+        <v>45.3</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>50</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>06-11-2025</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Северсталь</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>897739</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897739.html</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" t="n">
+        <v>4</v>
+      </c>
+      <c r="H27" t="n">
+        <v>5</v>
+      </c>
+      <c r="I27" t="n">
+        <v>19</v>
+      </c>
+      <c r="J27" t="n">
+        <v>37</v>
+      </c>
+      <c r="K27" t="n">
+        <v>56</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" t="n">
         <v>8</v>
       </c>
-      <c r="X21" t="n">
+      <c r="O27" t="n">
+        <v>2</v>
+      </c>
+      <c r="P27" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>29</v>
+      </c>
+      <c r="R27" t="n">
+        <v>14</v>
+      </c>
+      <c r="S27" t="n">
+        <v>9</v>
+      </c>
+      <c r="T27" t="n">
+        <v>33</v>
+      </c>
+      <c r="U27" t="n">
+        <v>10</v>
+      </c>
+      <c r="V27" t="n">
+        <v>10</v>
+      </c>
+      <c r="W27" t="n">
+        <v>8</v>
+      </c>
+      <c r="X27" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC27" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>04-11-2025</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Спартак</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>897729</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897729.html</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>29</v>
+      </c>
+      <c r="J28" t="n">
+        <v>33</v>
+      </c>
+      <c r="K28" t="n">
+        <v>62</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>8</v>
+      </c>
+      <c r="O28" t="n">
+        <v>8</v>
+      </c>
+      <c r="P28" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>25</v>
+      </c>
+      <c r="R28" t="n">
+        <v>23</v>
+      </c>
+      <c r="S28" t="n">
+        <v>10</v>
+      </c>
+      <c r="T28" t="n">
+        <v>38</v>
+      </c>
+      <c r="U28" t="n">
+        <v>31</v>
+      </c>
+      <c r="V28" t="n">
+        <v>4</v>
+      </c>
+      <c r="W28" t="n">
+        <v>9</v>
+      </c>
+      <c r="X28" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC28" t="n">
+        <v>47.9</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>55.1</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>02-11-2025</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Спартак</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>897723</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897723.html</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" t="n">
+        <v>30</v>
+      </c>
+      <c r="J29" t="n">
+        <v>50</v>
+      </c>
+      <c r="K29" t="n">
+        <v>80</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>10</v>
+      </c>
+      <c r="O29" t="n">
+        <v>8</v>
+      </c>
+      <c r="P29" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>38</v>
+      </c>
+      <c r="R29" t="n">
+        <v>14</v>
+      </c>
+      <c r="S29" t="n">
+        <v>5</v>
+      </c>
+      <c r="T29" t="n">
+        <v>39</v>
+      </c>
+      <c r="U29" t="n">
+        <v>30</v>
+      </c>
+      <c r="V29" t="n">
+        <v>4</v>
+      </c>
+      <c r="W29" t="n">
+        <v>5</v>
+      </c>
+      <c r="X29" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>17</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="AC29" t="n">
+        <v>45.7</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>22-10-2025</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Торпедо</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>897677</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897677.html</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>3</v>
+      </c>
+      <c r="I30" t="n">
+        <v>30</v>
+      </c>
+      <c r="J30" t="n">
+        <v>36</v>
+      </c>
+      <c r="K30" t="n">
+        <v>66</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>8</v>
+      </c>
+      <c r="O30" t="n">
+        <v>9</v>
+      </c>
+      <c r="P30" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>33</v>
+      </c>
+      <c r="R30" t="n">
+        <v>16</v>
+      </c>
+      <c r="S30" t="n">
+        <v>15</v>
+      </c>
+      <c r="T30" t="n">
+        <v>37</v>
+      </c>
+      <c r="U30" t="n">
+        <v>24</v>
+      </c>
+      <c r="V30" t="n">
+        <v>4</v>
+      </c>
+      <c r="W30" t="n">
+        <v>3</v>
+      </c>
+      <c r="X30" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>36</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC30" t="n">
+        <v>43.1</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>60.7</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>17-10-2025</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Автомобилист</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>897658</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897658.html</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2</v>
+      </c>
+      <c r="H31" t="n">
+        <v>3</v>
+      </c>
+      <c r="I31" t="n">
+        <v>22</v>
+      </c>
+      <c r="J31" t="n">
+        <v>34</v>
+      </c>
+      <c r="K31" t="n">
+        <v>56</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" t="n">
+        <v>10</v>
+      </c>
+      <c r="O31" t="n">
         <v>6</v>
       </c>
-      <c r="Y21" t="n">
-        <v>18</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>14</v>
-      </c>
-      <c r="AA21" t="n">
+      <c r="P31" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>32</v>
+      </c>
+      <c r="R31" t="n">
+        <v>13</v>
+      </c>
+      <c r="S31" t="n">
+        <v>11</v>
+      </c>
+      <c r="T31" t="n">
+        <v>30</v>
+      </c>
+      <c r="U31" t="n">
+        <v>23</v>
+      </c>
+      <c r="V31" t="n">
+        <v>2</v>
+      </c>
+      <c r="W31" t="n">
+        <v>3</v>
+      </c>
+      <c r="X31" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>43</v>
+      </c>
+      <c r="Z31" t="n">
         <v>4</v>
       </c>
-      <c r="AB21" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="AC21" t="n">
-        <v>28.3</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>58.3</v>
-      </c>
-      <c r="AE21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH21" t="n">
-        <v>4.8</v>
+      <c r="AA31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC31" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>56.6</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>9.1</v>
       </c>
     </row>
   </sheetData>
@@ -2894,7 +4025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3047,353 +4178,529 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>2.2</v>
+        <v>2.6</v>
       </c>
       <c r="D2" t="n">
-        <v>2.2</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8</v>
+        <v>-0.1</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="G2" t="n">
-        <v>27.6</v>
+        <v>33</v>
       </c>
       <c r="H2" t="n">
-        <v>25.3</v>
+        <v>15.5</v>
       </c>
       <c r="I2" t="n">
-        <v>-1.9</v>
+        <v>1.2</v>
       </c>
       <c r="J2" t="n">
-        <v>37.8</v>
+        <v>32.8</v>
       </c>
       <c r="K2" t="n">
-        <v>86.19999999999999</v>
+        <v>17.7</v>
       </c>
       <c r="L2" t="n">
-        <v>-3</v>
+        <v>-0.1</v>
       </c>
       <c r="M2" t="n">
-        <v>27.8</v>
+        <v>22.6</v>
       </c>
       <c r="N2" t="n">
-        <v>-3.6</v>
+        <v>-1</v>
       </c>
       <c r="O2" t="n">
-        <v>48.52</v>
+        <v>45.24</v>
       </c>
       <c r="P2" t="n">
-        <v>1.940000000000001</v>
+        <v>-2.090000000000001</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>-0.03299999999999999</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9</v>
+        <v>0.8699999999999999</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.08299999999999999</v>
+        <v>0.105</v>
       </c>
       <c r="U2" t="n">
-        <v>2.4</v>
+        <v>3.6</v>
       </c>
       <c r="V2" t="n">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="W2" t="n">
-        <v>12.2</v>
+        <v>8.6</v>
       </c>
       <c r="X2" t="n">
-        <v>-1.6</v>
+        <v>0.1</v>
       </c>
       <c r="Y2" t="n">
-        <v>7.8</v>
+        <v>8</v>
       </c>
       <c r="Z2" t="n">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="AA2" t="n">
-        <v>8.359999999999999</v>
+        <v>7.919999999999999</v>
       </c>
       <c r="AB2" t="n">
-        <v>3.74</v>
+        <v>-0.6799999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="D3" t="n">
-        <v>2.4</v>
+        <v>1.4</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.1</v>
+        <v>-1</v>
       </c>
       <c r="G3" t="n">
-        <v>31.8</v>
+        <v>23.4</v>
       </c>
       <c r="H3" t="n">
-        <v>29.7</v>
+        <v>72.8</v>
       </c>
       <c r="I3" t="n">
-        <v>-2.7</v>
+        <v>-3.2</v>
       </c>
       <c r="J3" t="n">
-        <v>30</v>
+        <v>27.8</v>
       </c>
       <c r="K3" t="n">
-        <v>111</v>
+        <v>27.7</v>
       </c>
       <c r="L3" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="M3" t="n">
-        <v>6.8</v>
+        <v>21.8</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.6</v>
+        <v>1.1</v>
       </c>
       <c r="O3" t="n">
-        <v>49.2</v>
+        <v>51.27999999999999</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4299999999999997</v>
+        <v>4.08</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1</v>
+        <v>0.258</v>
       </c>
       <c r="R3" t="n">
-        <v>0.025</v>
+        <v>-0.142</v>
       </c>
       <c r="S3" t="n">
-        <v>0.625</v>
+        <v>0.7</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.2833333333333333</v>
+        <v>0.25</v>
       </c>
       <c r="U3" t="n">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="V3" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="W3" t="n">
+        <v>16</v>
+      </c>
+      <c r="X3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="Z3" t="n">
         <v>1.6</v>
       </c>
-      <c r="W3" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>0.8</v>
-      </c>
       <c r="AA3" t="n">
-        <v>11.08</v>
+        <v>18.46</v>
       </c>
       <c r="AB3" t="n">
-        <v>3.57</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Спартак</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>5</v>
       </c>
       <c r="C4" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D4" t="n">
         <v>3.4</v>
       </c>
-      <c r="D4" t="n">
-        <v>3.8</v>
-      </c>
       <c r="E4" t="n">
-        <v>-0.7</v>
+        <v>-0.2</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2</v>
+        <v>0.5999999999999999</v>
       </c>
       <c r="G4" t="n">
-        <v>33.6</v>
+        <v>22.2</v>
       </c>
       <c r="H4" t="n">
-        <v>113.3</v>
+        <v>7.699999999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8</v>
+        <v>-0.8</v>
       </c>
       <c r="J4" t="n">
-        <v>27</v>
+        <v>34.8</v>
       </c>
       <c r="K4" t="n">
-        <v>40</v>
+        <v>48.7</v>
       </c>
       <c r="L4" t="n">
-        <v>-1.9</v>
+        <v>-2.5</v>
       </c>
       <c r="M4" t="n">
-        <v>17</v>
+        <v>21.2</v>
       </c>
       <c r="N4" t="n">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="O4" t="n">
-        <v>48.36</v>
+        <v>41.56</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.8799999999999997</v>
+        <v>-2.439999999999999</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.22</v>
+        <v>0.1175</v>
       </c>
       <c r="R4" t="n">
-        <v>0.02000000000000001</v>
+        <v>0.06633333333333334</v>
       </c>
       <c r="S4" t="n">
-        <v>0.77</v>
+        <v>0.8160000000000001</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.07100000000000001</v>
+        <v>-0.068</v>
       </c>
       <c r="U4" t="n">
-        <v>2.8</v>
+        <v>7</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.3</v>
+        <v>0.2</v>
       </c>
       <c r="W4" t="n">
-        <v>9.4</v>
+        <v>10</v>
       </c>
       <c r="X4" t="n">
-        <v>0.2</v>
+        <v>-0.6</v>
       </c>
       <c r="Y4" t="n">
-        <v>12.2</v>
+        <v>7.6</v>
       </c>
       <c r="Z4" t="n">
-        <v>-1</v>
+        <v>1.2</v>
       </c>
       <c r="AA4" t="n">
-        <v>10.2</v>
+        <v>12.58</v>
       </c>
       <c r="AB4" t="n">
-        <v>-2.33</v>
+        <v>-0.8699999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
       <c r="D5" t="n">
-        <v>2.2</v>
+        <v>1.6</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>25.2</v>
+        <v>31</v>
       </c>
       <c r="H5" t="n">
-        <v>33.7</v>
+        <v>31.5</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="J5" t="n">
-        <v>24.4</v>
+        <v>26</v>
       </c>
       <c r="K5" t="n">
-        <v>20.3</v>
+        <v>45</v>
       </c>
       <c r="L5" t="n">
-        <v>1.7</v>
+        <v>-3</v>
       </c>
       <c r="M5" t="n">
-        <v>16.4</v>
+        <v>23.2</v>
       </c>
       <c r="N5" t="n">
-        <v>4.1</v>
+        <v>0.2</v>
       </c>
       <c r="O5" t="n">
-        <v>45.34</v>
+        <v>58.02</v>
       </c>
       <c r="P5" t="n">
-        <v>-5.970000000000001</v>
+        <v>-0.08999999999999915</v>
       </c>
       <c r="Q5" t="n">
         <v>0.166</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.05</v>
+        <v>0.06699999999999999</v>
       </c>
       <c r="S5" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.784</v>
       </c>
       <c r="T5" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="U5" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="W5" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-0.4599999999999998</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Сибирь</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-2.6</v>
+      </c>
+      <c r="J6" t="n">
+        <v>40.6</v>
+      </c>
+      <c r="K6" t="n">
+        <v>46.8</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="M6" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O6" t="n">
+        <v>45.48</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-0.4700000000000003</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.1675</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-0.201</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.6279999999999999</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-0.074</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="W6" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="X6" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>7.56</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>-1.73</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ХК Сочи</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>26</v>
+      </c>
+      <c r="H7" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J7" t="n">
+        <v>38</v>
+      </c>
+      <c r="K7" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="M7" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="O7" t="n">
+        <v>45.38</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1.359999999999999</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.344</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-0.178</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.9099999999999999</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.01000000000000001</v>
+      </c>
+      <c r="U7" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="V7" t="n">
         <v>-0.1</v>
       </c>
-      <c r="U5" t="n">
-        <v>5</v>
-      </c>
-      <c r="V5" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="W5" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="X5" t="n">
-        <v>-1.2</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>6.959999999999999</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>1.09</v>
+      <c r="W7" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>10.04</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-2.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-12-16 15:07:52)
</commit_message>
<xml_diff>
--- a/khl/Form-5_Games_home_away.xlsx
+++ b/khl/Form-5_Games_home_away.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH81"/>
+  <dimension ref="A1:AH80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8808,7 +8808,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -8818,64 +8818,64 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>897837</v>
+        <v>897736</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897837.html</t>
+          <t>https://text.khl.ru/text/897736.html</t>
         </is>
       </c>
       <c r="F74" t="n">
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H74" t="n">
+        <v>1</v>
+      </c>
+      <c r="I74" t="n">
+        <v>20</v>
+      </c>
+      <c r="J74" t="n">
+        <v>29</v>
+      </c>
+      <c r="K74" t="n">
+        <v>49</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="n">
         <v>4</v>
       </c>
-      <c r="I74" t="n">
-        <v>29</v>
-      </c>
-      <c r="J74" t="n">
-        <v>24</v>
-      </c>
-      <c r="K74" t="n">
-        <v>53</v>
-      </c>
-      <c r="L74" t="n">
-        <v>0</v>
-      </c>
-      <c r="M74" t="n">
-        <v>2</v>
-      </c>
-      <c r="N74" t="n">
-        <v>8</v>
-      </c>
       <c r="O74" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P74" t="n">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="Q74" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="R74" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S74" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="T74" t="n">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="U74" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="V74" t="n">
         <v>1</v>
@@ -8884,45 +8884,45 @@
         <v>2</v>
       </c>
       <c r="X74" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y74" t="n">
+        <v>21</v>
+      </c>
+      <c r="Z74" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA74" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB74" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="AC74" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="AD74" t="n">
+        <v>48.1</v>
+      </c>
+      <c r="AE74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG74" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH74" t="n">
         <v>10</v>
-      </c>
-      <c r="Y74" t="n">
-        <v>17</v>
-      </c>
-      <c r="Z74" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA74" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB74" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="AC74" t="n">
-        <v>58.6</v>
-      </c>
-      <c r="AD74" t="n">
-        <v>77.09999999999999</v>
-      </c>
-      <c r="AE74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG74" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AH74" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -8932,129 +8932,129 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>897736</v>
+        <v>897728</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897736.html</t>
+          <t>https://text.khl.ru/text/897728.html</t>
         </is>
       </c>
       <c r="F75" t="n">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H75" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I75" t="n">
+        <v>39</v>
+      </c>
+      <c r="J75" t="n">
+        <v>25</v>
+      </c>
+      <c r="K75" t="n">
+        <v>64</v>
+      </c>
+      <c r="L75" t="n">
+        <v>2</v>
+      </c>
+      <c r="M75" t="n">
+        <v>2</v>
+      </c>
+      <c r="N75" t="n">
+        <v>6</v>
+      </c>
+      <c r="O75" t="n">
+        <v>12</v>
+      </c>
+      <c r="P75" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>29</v>
+      </c>
+      <c r="R75" t="n">
+        <v>8</v>
+      </c>
+      <c r="S75" t="n">
+        <v>23</v>
+      </c>
+      <c r="T75" t="n">
         <v>20</v>
       </c>
-      <c r="J75" t="n">
-        <v>29</v>
-      </c>
-      <c r="K75" t="n">
-        <v>49</v>
-      </c>
-      <c r="L75" t="n">
-        <v>0</v>
-      </c>
-      <c r="M75" t="n">
-        <v>0</v>
-      </c>
-      <c r="N75" t="n">
+      <c r="U75" t="n">
+        <v>12</v>
+      </c>
+      <c r="V75" t="n">
+        <v>3</v>
+      </c>
+      <c r="W75" t="n">
         <v>4</v>
       </c>
-      <c r="O75" t="n">
-        <v>6</v>
-      </c>
-      <c r="P75" t="n">
-        <v>27</v>
-      </c>
-      <c r="Q75" t="n">
-        <v>32</v>
-      </c>
-      <c r="R75" t="n">
+      <c r="X75" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y75" t="n">
         <v>19</v>
       </c>
-      <c r="S75" t="n">
-        <v>19</v>
-      </c>
-      <c r="T75" t="n">
-        <v>13</v>
-      </c>
-      <c r="U75" t="n">
-        <v>14</v>
-      </c>
-      <c r="V75" t="n">
-        <v>1</v>
-      </c>
-      <c r="W75" t="n">
-        <v>2</v>
-      </c>
-      <c r="X75" t="n">
-        <v>33</v>
-      </c>
-      <c r="Y75" t="n">
-        <v>21</v>
-      </c>
       <c r="Z75" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB75" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC75" t="n">
-        <v>45.8</v>
+        <v>59.2</v>
       </c>
       <c r="AD75" t="n">
-        <v>48.1</v>
+        <v>62.5</v>
       </c>
       <c r="AE75" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF75" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AG75" t="n">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="AH75" t="n">
-        <v>10</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Торпедо</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>897728</v>
+        <v>897860</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897728.html</t>
+          <t>https://text.khl.ru/text/897860.html</t>
         </is>
       </c>
       <c r="F76" t="n">
@@ -9064,93 +9064,93 @@
         <v>3</v>
       </c>
       <c r="H76" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I76" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="J76" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K76" t="n">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="L76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N76" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O76" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="P76" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="Q76" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="R76" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="S76" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="T76" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U76" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="V76" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W76" t="n">
+        <v>5</v>
+      </c>
+      <c r="X76" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y76" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z76" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA76" t="n">
         <v>4</v>
       </c>
-      <c r="X76" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y76" t="n">
-        <v>19</v>
-      </c>
-      <c r="Z76" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA76" t="n">
-        <v>1</v>
-      </c>
       <c r="AB76" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC76" t="n">
-        <v>59.2</v>
+        <v>62.5</v>
       </c>
       <c r="AD76" t="n">
-        <v>62.5</v>
+        <v>42.3</v>
       </c>
       <c r="AE76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF76" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="AG76" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AH76" t="n">
-        <v>7.7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -9160,15 +9160,15 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Трактор</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>897860</v>
+        <v>897850</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897860.html</t>
+          <t>https://text.khl.ru/text/897850.html</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -9178,64 +9178,64 @@
         <v>3</v>
       </c>
       <c r="H77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I77" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J77" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K77" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M77" t="n">
         <v>0</v>
       </c>
       <c r="N77" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O77" t="n">
         <v>8</v>
       </c>
       <c r="P77" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="Q77" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="R77" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="S77" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="T77" t="n">
+        <v>19</v>
+      </c>
+      <c r="U77" t="n">
         <v>22</v>
       </c>
-      <c r="U77" t="n">
-        <v>30</v>
-      </c>
       <c r="V77" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W77" t="n">
         <v>5</v>
       </c>
       <c r="X77" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Y77" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="Z77" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AA77" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AB77" t="inlineStr">
         <is>
@@ -9243,28 +9243,28 @@
         </is>
       </c>
       <c r="AC77" t="n">
-        <v>62.5</v>
+        <v>43.3</v>
       </c>
       <c r="AD77" t="n">
-        <v>42.3</v>
+        <v>46.3</v>
       </c>
       <c r="AE77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF77" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AG77" t="n">
         <v>1</v>
       </c>
       <c r="AH77" t="n">
-        <v>13</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -9274,111 +9274,111 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Трактор</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>897850</v>
+        <v>897798</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897850.html</t>
+          <t>https://text.khl.ru/text/897798.html</t>
         </is>
       </c>
       <c r="F78" t="n">
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H78" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I78" t="n">
+        <v>47</v>
+      </c>
+      <c r="J78" t="n">
         <v>19</v>
       </c>
-      <c r="J78" t="n">
-        <v>25</v>
-      </c>
       <c r="K78" t="n">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="L78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N78" t="n">
         <v>4</v>
       </c>
       <c r="O78" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P78" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="Q78" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="R78" t="n">
         <v>19</v>
       </c>
       <c r="S78" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="T78" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="U78" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="V78" t="n">
+        <v>5</v>
+      </c>
+      <c r="W78" t="n">
         <v>3</v>
       </c>
-      <c r="W78" t="n">
-        <v>5</v>
-      </c>
       <c r="X78" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="Y78" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="Z78" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB78" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC78" t="n">
-        <v>43.3</v>
+        <v>53.2</v>
       </c>
       <c r="AD78" t="n">
-        <v>46.3</v>
+        <v>53.6</v>
       </c>
       <c r="AE78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF78" t="n">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="AG78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH78" t="n">
-        <v>15.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -9388,111 +9388,111 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>897798</v>
+        <v>897786</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897798.html</t>
+          <t>https://text.khl.ru/text/897786.html</t>
         </is>
       </c>
       <c r="F79" t="n">
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H79" t="n">
+        <v>1</v>
+      </c>
+      <c r="I79" t="n">
+        <v>15</v>
+      </c>
+      <c r="J79" t="n">
+        <v>25</v>
+      </c>
+      <c r="K79" t="n">
+        <v>40</v>
+      </c>
+      <c r="L79" t="n">
+        <v>2</v>
+      </c>
+      <c r="M79" t="n">
+        <v>1</v>
+      </c>
+      <c r="N79" t="n">
+        <v>11</v>
+      </c>
+      <c r="O79" t="n">
+        <v>10</v>
+      </c>
+      <c r="P79" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>25</v>
+      </c>
+      <c r="R79" t="n">
+        <v>17</v>
+      </c>
+      <c r="S79" t="n">
+        <v>8</v>
+      </c>
+      <c r="T79" t="n">
+        <v>22</v>
+      </c>
+      <c r="U79" t="n">
+        <v>19</v>
+      </c>
+      <c r="V79" t="n">
+        <v>3</v>
+      </c>
+      <c r="W79" t="n">
         <v>5</v>
       </c>
-      <c r="I79" t="n">
-        <v>47</v>
-      </c>
-      <c r="J79" t="n">
-        <v>19</v>
-      </c>
-      <c r="K79" t="n">
-        <v>66</v>
-      </c>
-      <c r="L79" t="n">
-        <v>1</v>
-      </c>
-      <c r="M79" t="n">
-        <v>2</v>
-      </c>
-      <c r="N79" t="n">
-        <v>4</v>
-      </c>
-      <c r="O79" t="n">
-        <v>6</v>
-      </c>
-      <c r="P79" t="n">
-        <v>33</v>
-      </c>
-      <c r="Q79" t="n">
-        <v>29</v>
-      </c>
-      <c r="R79" t="n">
-        <v>19</v>
-      </c>
-      <c r="S79" t="n">
-        <v>27</v>
-      </c>
-      <c r="T79" t="n">
-        <v>15</v>
-      </c>
-      <c r="U79" t="n">
-        <v>13</v>
-      </c>
-      <c r="V79" t="n">
+      <c r="X79" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y79" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA79" t="n">
         <v>5</v>
       </c>
-      <c r="W79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X79" t="n">
-        <v>13</v>
-      </c>
-      <c r="Y79" t="n">
-        <v>11</v>
-      </c>
-      <c r="Z79" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA79" t="n">
-        <v>1</v>
-      </c>
       <c r="AB79" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC79" t="n">
-        <v>53.2</v>
+        <v>47.9</v>
       </c>
       <c r="AD79" t="n">
-        <v>53.6</v>
+        <v>53.7</v>
       </c>
       <c r="AE79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF79" t="n">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="AG79" t="n">
-        <v>0</v>
+        <v>0.82</v>
       </c>
       <c r="AH79" t="n">
-        <v>4.3</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -9502,218 +9502,104 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>897786</v>
+        <v>897777</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897786.html</t>
+          <t>https://text.khl.ru/text/897777.html</t>
         </is>
       </c>
       <c r="F80" t="n">
         <v>0</v>
       </c>
       <c r="G80" t="n">
+        <v>3</v>
+      </c>
+      <c r="H80" t="n">
         <v>4</v>
       </c>
-      <c r="H80" t="n">
-        <v>1</v>
-      </c>
       <c r="I80" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="J80" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K80" t="n">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="L80" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N80" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="O80" t="n">
+        <v>8</v>
+      </c>
+      <c r="P80" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>23</v>
+      </c>
+      <c r="R80" t="n">
+        <v>20</v>
+      </c>
+      <c r="S80" t="n">
+        <v>13</v>
+      </c>
+      <c r="T80" t="n">
+        <v>7</v>
+      </c>
+      <c r="U80" t="n">
         <v>10</v>
       </c>
-      <c r="P80" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q80" t="n">
-        <v>25</v>
-      </c>
-      <c r="R80" t="n">
-        <v>17</v>
-      </c>
-      <c r="S80" t="n">
-        <v>8</v>
-      </c>
-      <c r="T80" t="n">
-        <v>22</v>
-      </c>
-      <c r="U80" t="n">
-        <v>19</v>
-      </c>
       <c r="V80" t="n">
+        <v>2</v>
+      </c>
+      <c r="W80" t="n">
+        <v>1</v>
+      </c>
+      <c r="X80" t="n">
         <v>3</v>
       </c>
-      <c r="W80" t="n">
+      <c r="Y80" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z80" t="n">
         <v>5</v>
-      </c>
-      <c r="X80" t="n">
-        <v>18</v>
-      </c>
-      <c r="Y80" t="n">
-        <v>18</v>
-      </c>
-      <c r="Z80" t="n">
-        <v>3</v>
       </c>
       <c r="AA80" t="n">
         <v>5</v>
       </c>
       <c r="AB80" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC80" t="n">
-        <v>47.9</v>
+        <v>55.8</v>
       </c>
       <c r="AD80" t="n">
-        <v>53.7</v>
+        <v>41.2</v>
       </c>
       <c r="AE80" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF80" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AG80" t="n">
-        <v>0.82</v>
+        <v>0.33</v>
       </c>
       <c r="AH80" t="n">
-        <v>26.7</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>16-11-2025</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>ЦСКА</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Северсталь</t>
-        </is>
-      </c>
-      <c r="D81" t="n">
-        <v>897777</v>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>https://text.khl.ru/text/897777.html</t>
-        </is>
-      </c>
-      <c r="F81" t="n">
-        <v>0</v>
-      </c>
-      <c r="G81" t="n">
-        <v>3</v>
-      </c>
-      <c r="H81" t="n">
-        <v>4</v>
-      </c>
-      <c r="I81" t="n">
-        <v>27</v>
-      </c>
-      <c r="J81" t="n">
-        <v>22</v>
-      </c>
-      <c r="K81" t="n">
-        <v>49</v>
-      </c>
-      <c r="L81" t="n">
-        <v>0</v>
-      </c>
-      <c r="M81" t="n">
-        <v>2</v>
-      </c>
-      <c r="N81" t="n">
-        <v>6</v>
-      </c>
-      <c r="O81" t="n">
-        <v>8</v>
-      </c>
-      <c r="P81" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q81" t="n">
-        <v>23</v>
-      </c>
-      <c r="R81" t="n">
-        <v>20</v>
-      </c>
-      <c r="S81" t="n">
-        <v>13</v>
-      </c>
-      <c r="T81" t="n">
-        <v>7</v>
-      </c>
-      <c r="U81" t="n">
-        <v>10</v>
-      </c>
-      <c r="V81" t="n">
-        <v>2</v>
-      </c>
-      <c r="W81" t="n">
-        <v>1</v>
-      </c>
-      <c r="X81" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y81" t="n">
-        <v>13</v>
-      </c>
-      <c r="Z81" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA81" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB81" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="AC81" t="n">
-        <v>55.8</v>
-      </c>
-      <c r="AD81" t="n">
-        <v>41.2</v>
-      </c>
-      <c r="AE81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG81" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="AH81" t="n">
         <v>11.1</v>
       </c>
     </row>
@@ -11117,13 +11003,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="E16" t="n">
         <v>0.2</v>
@@ -11132,70 +11018,70 @@
         <v>0.3</v>
       </c>
       <c r="G16" t="n">
-        <v>29.8</v>
+        <v>30</v>
       </c>
       <c r="H16" t="n">
-        <v>60.7</v>
+        <v>80.66666666666667</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.1</v>
+        <v>-0.4</v>
       </c>
       <c r="J16" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K16" t="n">
-        <v>15.5</v>
+        <v>14</v>
       </c>
       <c r="L16" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
       <c r="M16" t="n">
-        <v>21.6</v>
+        <v>20.25</v>
       </c>
       <c r="N16" t="n">
-        <v>2.2</v>
+        <v>2.9</v>
       </c>
       <c r="O16" t="n">
-        <v>51.4</v>
+        <v>49.6</v>
       </c>
       <c r="P16" t="n">
-        <v>-2.740000000000001</v>
+        <v>-4.320000000000001</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.166</v>
+        <v>0.2075</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.01600000000000001</v>
+        <v>-0.049</v>
       </c>
       <c r="S16" t="n">
-        <v>0.5660000000000001</v>
+        <v>0.5825</v>
       </c>
       <c r="T16" t="n">
-        <v>0.034</v>
+        <v>0.101</v>
       </c>
       <c r="U16" t="n">
-        <v>2.2</v>
+        <v>2</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.2</v>
+        <v>-0.4</v>
       </c>
       <c r="W16" t="n">
-        <v>6.4</v>
+        <v>6</v>
       </c>
       <c r="X16" t="n">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="Y16" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="AA16" t="n">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.7200000000000001</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="17">

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-12-16 15:29:28)
</commit_message>
<xml_diff>
--- a/khl/Form-5_Games_home_away.xlsx
+++ b/khl/Form-5_Games_home_away.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH80"/>
+  <dimension ref="A1:AH81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8808,7 +8808,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -8818,64 +8818,64 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>897736</v>
+        <v>897837</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897736.html</t>
+          <t>https://text.khl.ru/text/897837.html</t>
         </is>
       </c>
       <c r="F74" t="n">
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I74" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="J74" t="n">
+        <v>24</v>
+      </c>
+      <c r="K74" t="n">
+        <v>53</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="n">
+        <v>2</v>
+      </c>
+      <c r="N74" t="n">
+        <v>8</v>
+      </c>
+      <c r="O74" t="n">
+        <v>4</v>
+      </c>
+      <c r="P74" t="n">
+        <v>41</v>
+      </c>
+      <c r="Q74" t="n">
         <v>29</v>
       </c>
-      <c r="K74" t="n">
-        <v>49</v>
-      </c>
-      <c r="L74" t="n">
-        <v>0</v>
-      </c>
-      <c r="M74" t="n">
-        <v>0</v>
-      </c>
-      <c r="N74" t="n">
-        <v>4</v>
-      </c>
-      <c r="O74" t="n">
-        <v>6</v>
-      </c>
-      <c r="P74" t="n">
+      <c r="R74" t="n">
+        <v>17</v>
+      </c>
+      <c r="S74" t="n">
+        <v>16</v>
+      </c>
+      <c r="T74" t="n">
         <v>27</v>
       </c>
-      <c r="Q74" t="n">
-        <v>32</v>
-      </c>
-      <c r="R74" t="n">
-        <v>19</v>
-      </c>
-      <c r="S74" t="n">
-        <v>19</v>
-      </c>
-      <c r="T74" t="n">
-        <v>13</v>
-      </c>
       <c r="U74" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="V74" t="n">
         <v>1</v>
@@ -8884,27 +8884,27 @@
         <v>2</v>
       </c>
       <c r="X74" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="Y74" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Z74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA74" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AB74" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC74" t="n">
-        <v>45.8</v>
+        <v>58.6</v>
       </c>
       <c r="AD74" t="n">
-        <v>48.1</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="AE74" t="n">
         <v>0</v>
@@ -8913,16 +8913,16 @@
         <v>0</v>
       </c>
       <c r="AG74" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH74" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -8932,129 +8932,129 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>897728</v>
+        <v>897736</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897728.html</t>
+          <t>https://text.khl.ru/text/897736.html</t>
         </is>
       </c>
       <c r="F75" t="n">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H75" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I75" t="n">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="J75" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K75" t="n">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="L75" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M75" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N75" t="n">
+        <v>4</v>
+      </c>
+      <c r="O75" t="n">
         <v>6</v>
       </c>
-      <c r="O75" t="n">
-        <v>12</v>
-      </c>
       <c r="P75" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="Q75" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="R75" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="S75" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="T75" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="U75" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="V75" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W75" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X75" t="n">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="Y75" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Z75" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AA75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB75" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC75" t="n">
-        <v>59.2</v>
+        <v>45.8</v>
       </c>
       <c r="AD75" t="n">
-        <v>62.5</v>
+        <v>48.1</v>
       </c>
       <c r="AE75" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF75" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="AG75" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AH75" t="n">
-        <v>7.7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Салават Юлаев</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>897860</v>
+        <v>897728</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897860.html</t>
+          <t>https://text.khl.ru/text/897728.html</t>
         </is>
       </c>
       <c r="F76" t="n">
@@ -9064,93 +9064,93 @@
         <v>3</v>
       </c>
       <c r="H76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I76" t="n">
+        <v>39</v>
+      </c>
+      <c r="J76" t="n">
+        <v>25</v>
+      </c>
+      <c r="K76" t="n">
+        <v>64</v>
+      </c>
+      <c r="L76" t="n">
+        <v>2</v>
+      </c>
+      <c r="M76" t="n">
+        <v>2</v>
+      </c>
+      <c r="N76" t="n">
+        <v>6</v>
+      </c>
+      <c r="O76" t="n">
+        <v>12</v>
+      </c>
+      <c r="P76" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>29</v>
+      </c>
+      <c r="R76" t="n">
+        <v>8</v>
+      </c>
+      <c r="S76" t="n">
         <v>23</v>
       </c>
-      <c r="J76" t="n">
-        <v>24</v>
-      </c>
-      <c r="K76" t="n">
-        <v>47</v>
-      </c>
-      <c r="L76" t="n">
-        <v>0</v>
-      </c>
-      <c r="M76" t="n">
-        <v>0</v>
-      </c>
-      <c r="N76" t="n">
+      <c r="T76" t="n">
+        <v>20</v>
+      </c>
+      <c r="U76" t="n">
+        <v>12</v>
+      </c>
+      <c r="V76" t="n">
+        <v>3</v>
+      </c>
+      <c r="W76" t="n">
+        <v>4</v>
+      </c>
+      <c r="X76" t="n">
         <v>8</v>
       </c>
-      <c r="O76" t="n">
-        <v>8</v>
-      </c>
-      <c r="P76" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q76" t="n">
-        <v>18</v>
-      </c>
-      <c r="R76" t="n">
-        <v>16</v>
-      </c>
-      <c r="S76" t="n">
-        <v>18</v>
-      </c>
-      <c r="T76" t="n">
-        <v>22</v>
-      </c>
-      <c r="U76" t="n">
-        <v>30</v>
-      </c>
-      <c r="V76" t="n">
-        <v>5</v>
-      </c>
-      <c r="W76" t="n">
-        <v>5</v>
-      </c>
-      <c r="X76" t="n">
-        <v>11</v>
-      </c>
       <c r="Y76" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="Z76" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AA76" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB76" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC76" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="AD76" t="n">
         <v>62.5</v>
       </c>
-      <c r="AD76" t="n">
-        <v>42.3</v>
-      </c>
       <c r="AE76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF76" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AG76" t="n">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="AH76" t="n">
-        <v>13</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -9160,15 +9160,15 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Трактор</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>897850</v>
+        <v>897860</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897850.html</t>
+          <t>https://text.khl.ru/text/897860.html</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -9178,64 +9178,64 @@
         <v>3</v>
       </c>
       <c r="H77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I77" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J77" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K77" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M77" t="n">
         <v>0</v>
       </c>
       <c r="N77" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O77" t="n">
         <v>8</v>
       </c>
       <c r="P77" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="Q77" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="R77" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="S77" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="T77" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="U77" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="V77" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W77" t="n">
         <v>5</v>
       </c>
       <c r="X77" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Y77" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Z77" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="AA77" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB77" t="inlineStr">
         <is>
@@ -9243,28 +9243,28 @@
         </is>
       </c>
       <c r="AC77" t="n">
-        <v>43.3</v>
+        <v>62.5</v>
       </c>
       <c r="AD77" t="n">
-        <v>46.3</v>
+        <v>42.3</v>
       </c>
       <c r="AE77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF77" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AG77" t="n">
         <v>1</v>
       </c>
       <c r="AH77" t="n">
-        <v>15.8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -9274,111 +9274,111 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>Трактор</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>897798</v>
+        <v>897850</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897798.html</t>
+          <t>https://text.khl.ru/text/897850.html</t>
         </is>
       </c>
       <c r="F78" t="n">
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H78" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I78" t="n">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="J78" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K78" t="n">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="L78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M78" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N78" t="n">
         <v>4</v>
       </c>
       <c r="O78" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P78" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="Q78" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="R78" t="n">
         <v>19</v>
       </c>
       <c r="S78" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="T78" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="U78" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="V78" t="n">
+        <v>3</v>
+      </c>
+      <c r="W78" t="n">
         <v>5</v>
       </c>
-      <c r="W78" t="n">
-        <v>3</v>
-      </c>
       <c r="X78" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Y78" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="Z78" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB78" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC78" t="n">
-        <v>53.2</v>
+        <v>43.3</v>
       </c>
       <c r="AD78" t="n">
-        <v>53.6</v>
+        <v>46.3</v>
       </c>
       <c r="AE78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF78" t="n">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AG78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH78" t="n">
-        <v>4.3</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -9388,111 +9388,111 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>897786</v>
+        <v>897798</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897786.html</t>
+          <t>https://text.khl.ru/text/897798.html</t>
         </is>
       </c>
       <c r="F79" t="n">
         <v>0</v>
       </c>
       <c r="G79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H79" t="n">
+        <v>5</v>
+      </c>
+      <c r="I79" t="n">
+        <v>47</v>
+      </c>
+      <c r="J79" t="n">
+        <v>19</v>
+      </c>
+      <c r="K79" t="n">
+        <v>66</v>
+      </c>
+      <c r="L79" t="n">
+        <v>1</v>
+      </c>
+      <c r="M79" t="n">
+        <v>2</v>
+      </c>
+      <c r="N79" t="n">
         <v>4</v>
       </c>
-      <c r="H79" t="n">
-        <v>1</v>
-      </c>
-      <c r="I79" t="n">
+      <c r="O79" t="n">
+        <v>6</v>
+      </c>
+      <c r="P79" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>29</v>
+      </c>
+      <c r="R79" t="n">
+        <v>19</v>
+      </c>
+      <c r="S79" t="n">
+        <v>27</v>
+      </c>
+      <c r="T79" t="n">
         <v>15</v>
       </c>
-      <c r="J79" t="n">
-        <v>25</v>
-      </c>
-      <c r="K79" t="n">
-        <v>40</v>
-      </c>
-      <c r="L79" t="n">
-        <v>2</v>
-      </c>
-      <c r="M79" t="n">
-        <v>1</v>
-      </c>
-      <c r="N79" t="n">
+      <c r="U79" t="n">
+        <v>13</v>
+      </c>
+      <c r="V79" t="n">
+        <v>5</v>
+      </c>
+      <c r="W79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X79" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y79" t="n">
         <v>11</v>
       </c>
-      <c r="O79" t="n">
-        <v>10</v>
-      </c>
-      <c r="P79" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q79" t="n">
-        <v>25</v>
-      </c>
-      <c r="R79" t="n">
-        <v>17</v>
-      </c>
-      <c r="S79" t="n">
-        <v>8</v>
-      </c>
-      <c r="T79" t="n">
-        <v>22</v>
-      </c>
-      <c r="U79" t="n">
-        <v>19</v>
-      </c>
-      <c r="V79" t="n">
-        <v>3</v>
-      </c>
-      <c r="W79" t="n">
-        <v>5</v>
-      </c>
-      <c r="X79" t="n">
-        <v>18</v>
-      </c>
-      <c r="Y79" t="n">
-        <v>18</v>
-      </c>
       <c r="Z79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA79" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB79" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC79" t="n">
-        <v>47.9</v>
+        <v>53.2</v>
       </c>
       <c r="AD79" t="n">
-        <v>53.7</v>
+        <v>53.6</v>
       </c>
       <c r="AE79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF79" t="n">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AG79" t="n">
-        <v>0.82</v>
+        <v>0</v>
       </c>
       <c r="AH79" t="n">
-        <v>26.7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -9502,104 +9502,218 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Северсталь</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>897777</v>
+        <v>897786</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897777.html</t>
+          <t>https://text.khl.ru/text/897786.html</t>
         </is>
       </c>
       <c r="F80" t="n">
         <v>0</v>
       </c>
       <c r="G80" t="n">
+        <v>4</v>
+      </c>
+      <c r="H80" t="n">
+        <v>1</v>
+      </c>
+      <c r="I80" t="n">
+        <v>15</v>
+      </c>
+      <c r="J80" t="n">
+        <v>25</v>
+      </c>
+      <c r="K80" t="n">
+        <v>40</v>
+      </c>
+      <c r="L80" t="n">
+        <v>2</v>
+      </c>
+      <c r="M80" t="n">
+        <v>1</v>
+      </c>
+      <c r="N80" t="n">
+        <v>11</v>
+      </c>
+      <c r="O80" t="n">
+        <v>10</v>
+      </c>
+      <c r="P80" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>25</v>
+      </c>
+      <c r="R80" t="n">
+        <v>17</v>
+      </c>
+      <c r="S80" t="n">
+        <v>8</v>
+      </c>
+      <c r="T80" t="n">
+        <v>22</v>
+      </c>
+      <c r="U80" t="n">
+        <v>19</v>
+      </c>
+      <c r="V80" t="n">
         <v>3</v>
       </c>
-      <c r="H80" t="n">
-        <v>4</v>
-      </c>
-      <c r="I80" t="n">
-        <v>27</v>
-      </c>
-      <c r="J80" t="n">
-        <v>22</v>
-      </c>
-      <c r="K80" t="n">
-        <v>49</v>
-      </c>
-      <c r="L80" t="n">
-        <v>0</v>
-      </c>
-      <c r="M80" t="n">
-        <v>2</v>
-      </c>
-      <c r="N80" t="n">
-        <v>6</v>
-      </c>
-      <c r="O80" t="n">
-        <v>8</v>
-      </c>
-      <c r="P80" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q80" t="n">
-        <v>23</v>
-      </c>
-      <c r="R80" t="n">
-        <v>20</v>
-      </c>
-      <c r="S80" t="n">
-        <v>13</v>
-      </c>
-      <c r="T80" t="n">
-        <v>7</v>
-      </c>
-      <c r="U80" t="n">
-        <v>10</v>
-      </c>
-      <c r="V80" t="n">
-        <v>2</v>
-      </c>
       <c r="W80" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="X80" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y80" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z80" t="n">
         <v>3</v>
-      </c>
-      <c r="Y80" t="n">
-        <v>13</v>
-      </c>
-      <c r="Z80" t="n">
-        <v>5</v>
       </c>
       <c r="AA80" t="n">
         <v>5</v>
       </c>
       <c r="AB80" t="inlineStr">
         <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="AC80" t="n">
+        <v>47.9</v>
+      </c>
+      <c r="AD80" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="AE80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF80" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AG80" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="AH80" t="n">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>16-11-2025</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ЦСКА</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Северсталь</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>897777</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>https://text.khl.ru/text/897777.html</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>3</v>
+      </c>
+      <c r="H81" t="n">
+        <v>4</v>
+      </c>
+      <c r="I81" t="n">
+        <v>27</v>
+      </c>
+      <c r="J81" t="n">
+        <v>22</v>
+      </c>
+      <c r="K81" t="n">
+        <v>49</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0</v>
+      </c>
+      <c r="M81" t="n">
+        <v>2</v>
+      </c>
+      <c r="N81" t="n">
+        <v>6</v>
+      </c>
+      <c r="O81" t="n">
+        <v>8</v>
+      </c>
+      <c r="P81" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>23</v>
+      </c>
+      <c r="R81" t="n">
+        <v>20</v>
+      </c>
+      <c r="S81" t="n">
+        <v>13</v>
+      </c>
+      <c r="T81" t="n">
+        <v>7</v>
+      </c>
+      <c r="U81" t="n">
+        <v>10</v>
+      </c>
+      <c r="V81" t="n">
+        <v>2</v>
+      </c>
+      <c r="W81" t="n">
+        <v>1</v>
+      </c>
+      <c r="X81" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y81" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z81" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA81" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB81" t="inlineStr">
+        <is>
           <t>L</t>
         </is>
       </c>
-      <c r="AC80" t="n">
+      <c r="AC81" t="n">
         <v>55.8</v>
       </c>
-      <c r="AD80" t="n">
+      <c r="AD81" t="n">
         <v>41.2</v>
       </c>
-      <c r="AE80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG80" t="n">
+      <c r="AE81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG81" t="n">
         <v>0.33</v>
       </c>
-      <c r="AH80" t="n">
+      <c r="AH81" t="n">
         <v>11.1</v>
       </c>
     </row>
@@ -11003,13 +11117,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D16" t="n">
         <v>3</v>
-      </c>
-      <c r="D16" t="n">
-        <v>2.75</v>
       </c>
       <c r="E16" t="n">
         <v>0.2</v>
@@ -11018,70 +11132,70 @@
         <v>0.3</v>
       </c>
       <c r="G16" t="n">
-        <v>30</v>
+        <v>29.8</v>
       </c>
       <c r="H16" t="n">
-        <v>80.66666666666667</v>
+        <v>60.7</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.4</v>
+        <v>-0.1</v>
       </c>
       <c r="J16" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K16" t="n">
-        <v>14</v>
+        <v>15.5</v>
       </c>
       <c r="L16" t="n">
-        <v>1.4</v>
+        <v>1.1</v>
       </c>
       <c r="M16" t="n">
-        <v>20.25</v>
+        <v>21.6</v>
       </c>
       <c r="N16" t="n">
-        <v>2.9</v>
+        <v>2.2</v>
       </c>
       <c r="O16" t="n">
-        <v>49.6</v>
+        <v>51.4</v>
       </c>
       <c r="P16" t="n">
-        <v>-4.320000000000001</v>
+        <v>-2.740000000000001</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.2075</v>
+        <v>0.166</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.049</v>
+        <v>-0.01600000000000001</v>
       </c>
       <c r="S16" t="n">
-        <v>0.5825</v>
+        <v>0.5660000000000001</v>
       </c>
       <c r="T16" t="n">
-        <v>0.101</v>
+        <v>0.034</v>
       </c>
       <c r="U16" t="n">
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="W16" t="n">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="X16" t="n">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="Y16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AA16" t="n">
-        <v>10.5</v>
+        <v>8.4</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.78</v>
+        <v>0.7200000000000001</v>
       </c>
     </row>
     <row r="17">

</xml_diff>